<commit_message>
fix any file name
</commit_message>
<xml_diff>
--- a/生徒名簿.xlsx
+++ b/生徒名簿.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eisu_Seat_manage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AAA464-9089-4FFF-9B9E-BCE88B3F1396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E655FD-6B85-4268-AAC8-8BBA73DD22D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9D5D34A-3ED5-431E-AE82-4EA5E6C77CE1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{D9D5D34A-3ED5-431E-AE82-4EA5E6C77CE1}"/>
   </bookViews>
   <sheets>
     <sheet name="小2" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="40">
   <si>
     <t>田中</t>
     <rPh sb="0" eb="2">
@@ -73,13 +73,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>本科</t>
-    <rPh sb="0" eb="2">
-      <t>ホンカ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>正田</t>
     <rPh sb="0" eb="2">
       <t>マサダ</t>
@@ -106,9 +99,6 @@
       <t>サイトウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>特講</t>
   </si>
   <si>
     <t>在籍番号</t>
@@ -259,6 +249,18 @@
   </si>
   <si>
     <t>2500002</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -628,21 +630,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB90CD49-6332-4985-A46C-6F6B912F5491}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -650,156 +652,156 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -814,20 +816,20 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:G9"/>
+      <selection activeCell="D2" sqref="D2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -835,114 +837,114 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -957,20 +959,20 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:G12"/>
+      <selection activeCell="D2" sqref="D2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -978,156 +980,156 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1142,20 +1144,20 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:G12"/>
+      <selection activeCell="D2" sqref="D2:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -1163,156 +1165,156 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1327,20 +1329,20 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="D2" sqref="D2:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -1348,156 +1350,156 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1510,21 +1512,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BD506A-5D0E-44F5-B68F-BB30D11F7EA5}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -1532,156 +1534,156 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>